<commit_message>
Duplicated column fixed. Column name corrected
</commit_message>
<xml_diff>
--- a/ProdutosUpdated.xlsx
+++ b/ProdutosUpdated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>Preço Base Reais</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Modificador Imposto</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -482,8 +477,9 @@
       <c r="D2" t="n">
         <v>1.1</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>1099.989</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -500,14 +496,11 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E3" t="n">
         <v>6750</v>
       </c>
-      <c r="F3" t="n">
-        <v>1.5</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -526,8 +519,9 @@
       <c r="D4" t="n">
         <v>1.1</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>989.9890000000001</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -544,14 +538,11 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E5" t="n">
         <v>1198.5</v>
       </c>
-      <c r="F5" t="n">
-        <v>1.5</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -570,8 +561,9 @@
       <c r="D6" t="n">
         <v>1.1</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>3300</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -588,14 +580,11 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E7" t="n">
         <v>720.72</v>
       </c>
-      <c r="F7" t="n">
-        <v>1.5</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -612,13 +601,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E8" t="n">
         <v>75</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>